<commit_message>
Attempt at new table reading, added to spreadsheet
</commit_message>
<xml_diff>
--- a/darpa_template.xlsx
+++ b/darpa_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isapoetzsch/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isapoetzsch/Documents/Utah 2020/GSoC/GSOC2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF2AA47-74B1-F342-BB47-F7BE27C661CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0241812B-9C83-494E-B912-10A3B9C762AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="78">
   <si>
     <t>Collection Name:</t>
   </si>
@@ -244,12 +244,73 @@
   <si>
     <t>Lac_Y</t>
   </si>
+  <si>
+    <t>This is a test collection.</t>
+  </si>
+  <si>
+    <t>Test collection</t>
+  </si>
+  <si>
+    <t>Isabel Pötzsch</t>
+  </si>
+  <si>
+    <t>Test Collection</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>pT7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">taatacgact cactataggg aga </t>
+  </si>
+  <si>
+    <t>tetR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">atgtccagat tagataaaag taaagtgatt aacagcgcat tagagctgcttaatgaggtc ggaatcgaag gtttaacaac ccgtaaactc gcccagaagc
+taggtgtaga gcagcctaca ttgtattggc atgtaaaaaa taagcgggct ttgctcgacg ccttagccat tgagatgtta gataggcacc atactcactt ttgcccttta gaaggggaaa gctggcaaga ttttttacgt aataacgcta
+aaagttttag atgtgcttta ctaagtcatc gcgatggagc aaaagtacat ttaggtacac ggcctacaga aaaacagtat gaaactctcg aaaatcaattagccttttta tgccaacaag gtttttcact agagaatgca ttatatgcac tcagcgctgt ggggcatttt actttaggtt gcgtattgga agatcaagag
+catcaagtcg ctaaagaaga aagggaaaca cctactactg atagtatgccgccattatta cgacaagcta tcgaattatt tgatcaccaa ggtgcagagccagccttctt attcggcctt gaattgatca tatgcggatt agaaaaacaacttaaatgtg aaagtgggtc cgctgcaaac gacgaaaact acgctttagt
+agcttaataa cactgatagt gctagtgtag atcac </t>
+  </si>
+  <si>
+    <t>M36010</t>
+  </si>
+  <si>
+    <t>E. coli RNA pol transcription terminator designed and tested by Guillaume Cambray at BIOFAB Emeryville. Based on the natural E. coli rnpB T1 terminator.</t>
+  </si>
+  <si>
+    <t>tcggtcagtt tcacctgatt tacgtaaaaa cccgcttcgg cgggtttttgcttttggagg ggcagaaaga tgaatgactg tc</t>
+  </si>
+  <si>
+    <t>Just a T7 Promoter</t>
+  </si>
+  <si>
+    <t>Coding region for the TetR protein without the Ribosome Binding Site. Modified with an LVA tail for rapid degradation of the protein and faster fall time for the emission. TetR binds to the pTet regulator (BBa_R0040). aTc (anhydrotetracycline) binds to TetR and inhibits its operation.</t>
+  </si>
+  <si>
+    <t>Lactose transport receptor</t>
+  </si>
+  <si>
+    <t>green fluorescent protein derived from jellyfish Aequeora victoria wild-type GFP (SwissProt: P42212</t>
+  </si>
+  <si>
+    <t>Description A</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -307,6 +368,18 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF333333"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -534,7 +607,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -586,7 +659,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -595,6 +671,11 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -813,7 +894,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D8"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -831,7 +912,9 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="36" t="s">
+        <v>60</v>
+      </c>
       <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
@@ -847,7 +930,9 @@
       <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="37">
+        <v>44001</v>
+      </c>
       <c r="D3" s="5"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -861,7 +946,9 @@
       <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="36" t="s">
+        <v>61</v>
+      </c>
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -882,7 +969,9 @@
       <c r="A8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="36" t="s">
+        <v>60</v>
+      </c>
       <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -923,11 +1012,13 @@
       <c r="E10" s="10"/>
     </row>
     <row r="11" spans="1:26" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="35"/>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="37"/>
+      <c r="A11" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="39"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="40"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -985,7 +1076,10 @@
         <v>55</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>76</v>
       </c>
       <c r="E15">
         <v>720</v>
@@ -999,7 +1093,10 @@
         <v>58</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
+      </c>
+      <c r="C16" s="35" t="s">
+        <v>75</v>
       </c>
       <c r="E16" s="32">
         <v>1288</v>
@@ -1008,69 +1105,108 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="2"/>
-      <c r="F17" s="15"/>
-    </row>
-    <row r="18" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="2"/>
-      <c r="F18" s="15"/>
-    </row>
-    <row r="19" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="2"/>
-      <c r="F19" s="32"/>
-    </row>
-    <row r="20" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17">
+        <v>23</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" s="35">
+        <v>685</v>
+      </c>
+      <c r="F18" s="33" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" s="35">
+        <v>82</v>
+      </c>
+      <c r="F19" s="43" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="2"/>
-      <c r="F20" s="32"/>
-    </row>
-    <row r="21" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F20" s="43"/>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="2"/>
       <c r="F21" s="16"/>
     </row>
-    <row r="22" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="2"/>
       <c r="F22" s="17"/>
     </row>
-    <row r="23" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="2"/>
-      <c r="F23" s="32"/>
-    </row>
-    <row r="24" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F23" s="35"/>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="2"/>
-      <c r="F24" s="32"/>
-    </row>
-    <row r="25" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F24" s="35"/>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="2"/>
       <c r="F25" s="16"/>
     </row>
-    <row r="26" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="2"/>
       <c r="F26" s="17"/>
     </row>
-    <row r="27" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="2"/>
-      <c r="F27" s="32"/>
-    </row>
-    <row r="28" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F27" s="35"/>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="2"/>
-      <c r="F28" s="32"/>
-    </row>
-    <row r="29" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F28" s="35"/>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="2"/>
-      <c r="F29" s="32"/>
-    </row>
-    <row r="30" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F29" s="35"/>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="2"/>
       <c r="C30" s="9"/>
-      <c r="F30" s="32"/>
-    </row>
-    <row r="31" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F30" s="35"/>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="2"/>
       <c r="C31" s="9"/>
-      <c r="F31" s="32"/>
-    </row>
-    <row r="32" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F31" s="35"/>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="2"/>
       <c r="C32" s="9"/>
       <c r="F32" s="32"/>
@@ -2174,8 +2310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{733B2DFE-EFBF-0640-98AB-35CC018B7763}">
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2187,7 +2323,9 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="36" t="s">
+        <v>62</v>
+      </c>
       <c r="C1" s="34"/>
       <c r="D1" s="5" t="s">
         <v>3</v>
@@ -2263,7 +2401,9 @@
       <c r="A18" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="19"/>
+      <c r="B18" s="19">
+        <v>1</v>
+      </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
@@ -2273,9 +2413,15 @@
       <c r="A19" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
+      <c r="B19" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>65</v>
+      </c>
       <c r="E19" s="21"/>
       <c r="F19" s="22"/>
     </row>
@@ -2283,7 +2429,9 @@
       <c r="A20" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="24"/>
+      <c r="B20" s="45" t="s">
+        <v>77</v>
+      </c>
       <c r="C20" s="25"/>
       <c r="D20" s="25"/>
       <c r="E20" s="25"/>
@@ -2313,40 +2461,48 @@
       <c r="A23" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="9"/>
+      <c r="B23" s="44" t="s">
+        <v>66</v>
+      </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="38" t="s">
+      <c r="A24" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="9"/>
+      <c r="B24" s="44" t="s">
+        <v>55</v>
+      </c>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="39"/>
-      <c r="B25" s="9"/>
+      <c r="A25" s="42"/>
+      <c r="B25" s="44" t="s">
+        <v>68</v>
+      </c>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="39"/>
-      <c r="B26" s="9"/>
+      <c r="A26" s="42"/>
+      <c r="B26" s="35" t="s">
+        <v>70</v>
+      </c>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="39"/>
+      <c r="A27" s="42"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
@@ -2379,7 +2535,9 @@
       <c r="A32" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="19"/>
+      <c r="B32" s="19">
+        <v>2</v>
+      </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -2482,7 +2640,9 @@
       <c r="A46" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B46" s="19"/>
+      <c r="B46" s="19">
+        <v>3</v>
+      </c>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
@@ -2652,7 +2812,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Updated spreadsheet and output files
</commit_message>
<xml_diff>
--- a/darpa_template.xlsx
+++ b/darpa_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isapoetzsch/Documents/Utah 2020/GSoC/GSOC2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0241812B-9C83-494E-B912-10A3B9C762AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61796769-E10C-574B-BA51-D08D366E2171}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="80">
   <si>
     <t>Collection Name:</t>
   </si>
@@ -189,9 +189,6 @@
   </si>
   <si>
     <t>Add parts for each composite in a vertical list, from 5' top to 3' bottom; you can add more rows and more collections if you need</t>
-  </si>
-  <si>
-    <t>Parts:</t>
   </si>
   <si>
     <t>GFP</t>
@@ -304,6 +301,15 @@
   </si>
   <si>
     <t>Description A</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Libraries</t>
+  </si>
+  <si>
+    <t>https://synbiohub.org/public/igem/igem_collection/1</t>
   </si>
 </sst>
 </file>
@@ -607,7 +613,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -662,6 +668,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -671,11 +683,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -894,7 +902,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -913,7 +921,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>3</v>
@@ -947,7 +955,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D5" s="5"/>
     </row>
@@ -970,7 +978,7 @@
         <v>16</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D8" s="5"/>
     </row>
@@ -1012,13 +1020,13 @@
       <c r="E10" s="10"/>
     </row>
     <row r="11" spans="1:26" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="40"/>
+      <c r="A11" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="43"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="44"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1073,92 +1081,92 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="35" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E15">
         <v>720</v>
       </c>
       <c r="F15" s="33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E16" s="32">
         <v>1288</v>
       </c>
       <c r="F16" s="33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E17">
         <v>23</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E18" s="35">
         <v>685</v>
       </c>
       <c r="F18" s="33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C19" s="35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E19" s="35">
         <v>82</v>
       </c>
-      <c r="F19" s="43" t="s">
-        <v>72</v>
+      <c r="F19" s="38" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="2"/>
-      <c r="F20" s="43"/>
+      <c r="F20" s="38"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="2"/>
@@ -2308,10 +2316,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{733B2DFE-EFBF-0640-98AB-35CC018B7763}">
-  <dimension ref="A1:F66"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2324,7 +2332,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C1" s="34"/>
       <c r="D1" s="5" t="s">
@@ -2386,6 +2394,14 @@
       <c r="B8" s="3"/>
       <c r="C8" s="34"/>
       <c r="D8" s="5"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="41" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
@@ -2414,13 +2430,13 @@
         <v>48</v>
       </c>
       <c r="B19" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="D19" s="21" t="s">
         <v>64</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>65</v>
       </c>
       <c r="E19" s="21"/>
       <c r="F19" s="22"/>
@@ -2429,8 +2445,8 @@
       <c r="A20" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="45" t="s">
-        <v>77</v>
+      <c r="B20" s="40" t="s">
+        <v>76</v>
       </c>
       <c r="C20" s="25"/>
       <c r="D20" s="25"/>
@@ -2461,8 +2477,8 @@
       <c r="A23" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="44" t="s">
-        <v>66</v>
+      <c r="B23" s="39" t="s">
+        <v>65</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
@@ -2470,11 +2486,11 @@
       <c r="F23" s="9"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="41" t="s">
+      <c r="A24" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="44" t="s">
-        <v>55</v>
+      <c r="B24" s="39" t="s">
+        <v>54</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
@@ -2482,9 +2498,9 @@
       <c r="F24" s="9"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="42"/>
-      <c r="B25" s="44" t="s">
-        <v>68</v>
+      <c r="A25" s="46"/>
+      <c r="B25" s="39" t="s">
+        <v>67</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
@@ -2492,9 +2508,9 @@
       <c r="F25" s="9"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="42"/>
+      <c r="A26" s="46"/>
       <c r="B26" s="35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
@@ -2502,7 +2518,7 @@
       <c r="F26" s="9"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="42"/>
+      <c r="A27" s="46"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
@@ -2745,7 +2761,9 @@
       <c r="A61" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B61" s="19"/>
+      <c r="B61" s="19">
+        <v>4</v>
+      </c>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
@@ -2793,12 +2811,29 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="B66" s="9"/>
+        <v>52</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="C66" s="9"/>
       <c r="D66" s="9"/>
       <c r="E66" s="15"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B67" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B68" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B69" t="s">
+        <v>77</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Added library abbreviation field
</commit_message>
<xml_diff>
--- a/darpa_template.xlsx
+++ b/darpa_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isapoetzsch/Documents/Utah 2020/GSoC/GSOC2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61796769-E10C-574B-BA51-D08D366E2171}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E9EEC6-E4B5-9649-A02E-05A752D8DA01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="87">
   <si>
     <t>Collection Name:</t>
   </si>
@@ -311,12 +311,33 @@
   <si>
     <t>https://synbiohub.org/public/igem/igem_collection/1</t>
   </si>
+  <si>
+    <t>Add libraries in a horizontal list</t>
+  </si>
+  <si>
+    <t>Abbreviations</t>
+  </si>
+  <si>
+    <t>igem</t>
+  </si>
+  <si>
+    <t>A_1</t>
+  </si>
+  <si>
+    <t>B_1</t>
+  </si>
+  <si>
+    <t>C_1</t>
+  </si>
+  <si>
+    <t>D_1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -389,8 +410,36 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -409,8 +458,14 @@
         <bgColor rgb="FFE2EFD9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2F0D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -609,11 +664,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -637,7 +731,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -679,17 +772,28 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFE2F0D9"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -920,7 +1024,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="35" t="s">
         <v>59</v>
       </c>
       <c r="D1" s="5" t="s">
@@ -938,7 +1042,7 @@
       <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="37">
+      <c r="B3" s="36">
         <v>44001</v>
       </c>
       <c r="D3" s="5"/>
@@ -954,7 +1058,7 @@
       <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="35" t="s">
         <v>60</v>
       </c>
       <c r="D5" s="5"/>
@@ -977,7 +1081,7 @@
       <c r="A8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="35" t="s">
         <v>59</v>
       </c>
       <c r="D8" s="5"/>
@@ -1020,13 +1124,13 @@
       <c r="E10" s="10"/>
     </row>
     <row r="11" spans="1:26" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="43"/>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="44"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="43"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1086,41 +1190,41 @@
       <c r="B15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="34" t="s">
         <v>75</v>
       </c>
       <c r="E15">
         <v>720</v>
       </c>
-      <c r="F15" s="33" t="s">
+      <c r="F15" s="32" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="31" t="s">
         <v>57</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="35" t="s">
+      <c r="C16" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="E16" s="32">
+      <c r="E16" s="31">
         <v>1288</v>
       </c>
-      <c r="F16" s="33" t="s">
+      <c r="F16" s="32" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="34" t="s">
         <v>65</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="35" t="s">
+      <c r="C17" s="34" t="s">
         <v>72</v>
       </c>
       <c r="E17">
@@ -1131,42 +1235,42 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="34" t="s">
         <v>67</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="35" t="s">
+      <c r="C18" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="35">
+      <c r="E18" s="34">
         <v>685</v>
       </c>
-      <c r="F18" s="33" t="s">
+      <c r="F18" s="32" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="34" t="s">
         <v>69</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="35" t="s">
+      <c r="C19" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="E19" s="35">
+      <c r="E19" s="34">
         <v>82</v>
       </c>
-      <c r="F19" s="38" t="s">
+      <c r="F19" s="37" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="2"/>
-      <c r="F20" s="38"/>
+      <c r="F20" s="37"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="2"/>
@@ -1178,11 +1282,11 @@
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="2"/>
-      <c r="F23" s="35"/>
+      <c r="F23" s="34"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="2"/>
-      <c r="F24" s="35"/>
+      <c r="F24" s="34"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="2"/>
@@ -1194,60 +1298,60 @@
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="2"/>
-      <c r="F27" s="35"/>
+      <c r="F27" s="34"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="2"/>
-      <c r="F28" s="35"/>
+      <c r="F28" s="34"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="2"/>
-      <c r="F29" s="35"/>
+      <c r="F29" s="34"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="2"/>
       <c r="C30" s="9"/>
-      <c r="F30" s="35"/>
+      <c r="F30" s="34"/>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="2"/>
       <c r="C31" s="9"/>
-      <c r="F31" s="35"/>
+      <c r="F31" s="34"/>
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="2"/>
       <c r="C32" s="9"/>
-      <c r="F32" s="32"/>
+      <c r="F32" s="31"/>
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="2"/>
       <c r="C33" s="9"/>
-      <c r="F33" s="32"/>
+      <c r="F33" s="31"/>
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="2"/>
       <c r="C34" s="9"/>
-      <c r="F34" s="32"/>
+      <c r="F34" s="31"/>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="2"/>
       <c r="C35" s="9"/>
-      <c r="F35" s="32"/>
+      <c r="F35" s="31"/>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="2"/>
       <c r="C36" s="9"/>
-      <c r="F36" s="32"/>
+      <c r="F36" s="31"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="2"/>
       <c r="C37" s="9"/>
-      <c r="F37" s="32"/>
+      <c r="F37" s="31"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="2"/>
       <c r="C38" s="9"/>
-      <c r="F38" s="32"/>
+      <c r="F38" s="31"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="18"/>
@@ -2319,7 +2423,7 @@
   <dimension ref="A1:F69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2327,81 +2431,108 @@
     <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="34"/>
+      <c r="C1" s="33"/>
       <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="34"/>
+      <c r="C2" s="33"/>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="34"/>
+      <c r="C3" s="33"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="34"/>
+      <c r="C4" s="33"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="34"/>
+      <c r="C5" s="33"/>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="3"/>
-      <c r="C6" s="34"/>
+      <c r="C6" s="33"/>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="3"/>
-      <c r="C7" s="34"/>
+      <c r="C7" s="33"/>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="3"/>
-      <c r="C8" s="34"/>
+      <c r="C8" s="33"/>
       <c r="D8" s="5"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="47" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="48" t="s">
         <v>79</v>
       </c>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+    </row>
+    <row r="11" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="50" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="51" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="46" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="40"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="40"/>
     </row>
     <row r="17" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
@@ -2417,8 +2548,8 @@
       <c r="A18" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="19">
-        <v>1</v>
+      <c r="B18" s="52" t="s">
+        <v>83</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -2429,55 +2560,55 @@
       <c r="A19" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="D19" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="E19" s="21"/>
-      <c r="F19" s="22"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="21"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="23" t="s">
+      <c r="A20" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="26"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="25"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="29"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="28"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="27" t="s">
+      <c r="A22" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
       <c r="F22" s="3"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="39" t="s">
+      <c r="B23" s="38" t="s">
         <v>65</v>
       </c>
       <c r="C23" s="9"/>
@@ -2489,7 +2620,7 @@
       <c r="A24" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="39" t="s">
+      <c r="B24" s="38" t="s">
         <v>54</v>
       </c>
       <c r="C24" s="9"/>
@@ -2498,8 +2629,8 @@
       <c r="F24" s="9"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="46"/>
-      <c r="B25" s="39" t="s">
+      <c r="A25" s="44"/>
+      <c r="B25" s="38" t="s">
         <v>67</v>
       </c>
       <c r="C25" s="9"/>
@@ -2508,8 +2639,8 @@
       <c r="F25" s="9"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="46"/>
-      <c r="B26" s="35" t="s">
+      <c r="A26" s="44"/>
+      <c r="B26" s="34" t="s">
         <v>69</v>
       </c>
       <c r="C26" s="9"/>
@@ -2518,7 +2649,7 @@
       <c r="F26" s="9"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="46"/>
+      <c r="A27" s="44"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
@@ -2548,11 +2679,11 @@
       <c r="F30" s="18"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="19">
-        <v>2</v>
+      <c r="B32" s="52" t="s">
+        <v>84</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
@@ -2563,44 +2694,44 @@
       <c r="A33" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="20"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="22"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="21"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="23" t="s">
+      <c r="A34" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="24"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="26"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="25"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="27" t="s">
+      <c r="A35" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="B35" s="28"/>
-      <c r="C35" s="28"/>
-      <c r="D35" s="28"/>
-      <c r="E35" s="28"/>
-      <c r="F35" s="29"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="28"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="27" t="s">
+      <c r="A36" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="B36" s="30"/>
-      <c r="C36" s="30"/>
-      <c r="D36" s="30"/>
-      <c r="E36" s="30"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="29"/>
       <c r="F36" s="3"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="31" t="s">
+      <c r="A37" s="30" t="s">
         <v>52</v>
       </c>
       <c r="B37" s="9"/>
@@ -2653,11 +2784,11 @@
       <c r="F44" s="18"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="31" t="s">
+      <c r="A46" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B46" s="19">
-        <v>3</v>
+      <c r="B46" s="52" t="s">
+        <v>85</v>
       </c>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
@@ -2668,44 +2799,44 @@
       <c r="A47" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B47" s="20"/>
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
-      <c r="E47" s="21"/>
-      <c r="F47" s="22"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="21"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="23" t="s">
+      <c r="A48" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="B48" s="24"/>
-      <c r="C48" s="25"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="25"/>
-      <c r="F48" s="26"/>
+      <c r="B48" s="23"/>
+      <c r="C48" s="24"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="25"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="27" t="s">
+      <c r="A49" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="B49" s="28"/>
-      <c r="C49" s="28"/>
-      <c r="D49" s="28"/>
-      <c r="E49" s="28"/>
-      <c r="F49" s="29"/>
+      <c r="B49" s="27"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="27"/>
+      <c r="E49" s="27"/>
+      <c r="F49" s="28"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="27" t="s">
+      <c r="A50" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="B50" s="30"/>
-      <c r="C50" s="30"/>
-      <c r="D50" s="30"/>
-      <c r="E50" s="30"/>
+      <c r="B50" s="29"/>
+      <c r="C50" s="29"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="29"/>
       <c r="F50" s="3"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="31" t="s">
+      <c r="A51" s="30" t="s">
         <v>52</v>
       </c>
       <c r="B51" s="9"/>
@@ -2758,11 +2889,11 @@
       <c r="F59" s="18"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="31" t="s">
+      <c r="A61" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B61" s="19">
-        <v>4</v>
+      <c r="B61" s="52" t="s">
+        <v>86</v>
       </c>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
@@ -2773,44 +2904,44 @@
       <c r="A62" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B62" s="20"/>
-      <c r="C62" s="21"/>
-      <c r="D62" s="21"/>
-      <c r="E62" s="21"/>
-      <c r="F62" s="22"/>
+      <c r="B62" s="19"/>
+      <c r="C62" s="20"/>
+      <c r="D62" s="20"/>
+      <c r="E62" s="20"/>
+      <c r="F62" s="21"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="23" t="s">
+      <c r="A63" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="B63" s="24"/>
-      <c r="C63" s="25"/>
-      <c r="D63" s="25"/>
-      <c r="E63" s="25"/>
-      <c r="F63" s="26"/>
+      <c r="B63" s="23"/>
+      <c r="C63" s="24"/>
+      <c r="D63" s="24"/>
+      <c r="E63" s="24"/>
+      <c r="F63" s="25"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" s="27" t="s">
+      <c r="A64" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="B64" s="28"/>
-      <c r="C64" s="28"/>
-      <c r="D64" s="28"/>
-      <c r="E64" s="28"/>
-      <c r="F64" s="29"/>
+      <c r="B64" s="27"/>
+      <c r="C64" s="27"/>
+      <c r="D64" s="27"/>
+      <c r="E64" s="27"/>
+      <c r="F64" s="28"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="27" t="s">
+      <c r="A65" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="B65" s="30"/>
-      <c r="C65" s="30"/>
-      <c r="D65" s="30"/>
-      <c r="E65" s="30"/>
+      <c r="B65" s="29"/>
+      <c r="C65" s="29"/>
+      <c r="D65" s="29"/>
+      <c r="E65" s="29"/>
       <c r="F65" s="3"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="31" t="s">
+      <c r="A66" s="30" t="s">
         <v>52</v>
       </c>
       <c r="B66" s="2" t="s">

</xml_diff>

<commit_message>
Replacement for invalid collection names
</commit_message>
<xml_diff>
--- a/darpa_template.xlsx
+++ b/darpa_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isapoetzsch/Documents/Utah_2020/GSoC/GSOC2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E740AE-F67F-F543-A718-ACFEB556B2D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53BA098-CE66-CC48-A810-82AA274ADB15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -329,9 +329,6 @@
     <t>D_1</t>
   </si>
   <si>
-    <t>https://synbiohub.org/public/bsu/bsu_collection/1</t>
-  </si>
-  <si>
     <t>Add libraries in a vertical list and add more rows if necessary</t>
   </si>
   <si>
@@ -356,13 +353,16 @@
     <t>C_24</t>
   </si>
   <si>
-    <t>A_1%</t>
-  </si>
-  <si>
     <t>https://synbiohub.org/public/igem</t>
   </si>
   <si>
     <t>BBa_M36010</t>
+  </si>
+  <si>
+    <t>https://synbiohub.org/public/bsu</t>
+  </si>
+  <si>
+    <t>A_1%Äñ</t>
   </si>
 </sst>
 </file>
@@ -755,7 +755,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -816,7 +816,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -825,6 +824,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -834,8 +835,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -1178,13 +1177,13 @@
       <c r="E10" s="10"/>
     </row>
     <row r="11" spans="1:26" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="52" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="52"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="53"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="54"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2477,7 +2476,7 @@
   <dimension ref="A1:N66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2554,14 +2553,14 @@
       <c r="D8" s="5"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="47" t="s">
-        <v>84</v>
+      <c r="C10" s="46" t="s">
+        <v>83</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -2569,13 +2568,13 @@
       <c r="N10" s="41"/>
     </row>
     <row r="11" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="56" t="s">
-        <v>93</v>
-      </c>
-      <c r="B11" s="43" t="s">
+      <c r="A11" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="C11" s="49"/>
+      <c r="C11" s="48"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
@@ -2584,29 +2583,29 @@
       <c r="N11" s="40"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="42" t="s">
-        <v>83</v>
-      </c>
-      <c r="B12" s="48" t="s">
-        <v>85</v>
-      </c>
-      <c r="C12" s="49"/>
+      <c r="A12" s="50" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="48"/>
       <c r="L12" s="40"/>
       <c r="M12" s="40"/>
       <c r="N12" s="40"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="48"/>
-      <c r="B13" s="50"/>
-      <c r="C13" s="49"/>
+      <c r="A13" s="47"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="48"/>
       <c r="L13" s="40"/>
       <c r="M13" s="40"/>
       <c r="N13" s="40"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="48"/>
-      <c r="B14" s="48"/>
-      <c r="C14" s="49"/>
+      <c r="A14" s="47"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="48"/>
       <c r="L14" s="40"/>
       <c r="M14" s="40"/>
       <c r="N14" s="40"/>
@@ -2630,8 +2629,8 @@
       <c r="A18" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="44" t="s">
-        <v>92</v>
+      <c r="B18" s="43" t="s">
+        <v>94</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -2691,7 +2690,7 @@
         <v>52</v>
       </c>
       <c r="B23" s="38" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
@@ -2699,11 +2698,11 @@
       <c r="F23" s="9"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="54" t="s">
+      <c r="A24" s="55" t="s">
         <v>53</v>
       </c>
       <c r="B24" s="38" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
@@ -2711,9 +2710,9 @@
       <c r="F24" s="9"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="55"/>
+      <c r="A25" s="56"/>
       <c r="B25" s="38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
@@ -2721,9 +2720,9 @@
       <c r="F25" s="9"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="55"/>
+      <c r="A26" s="56"/>
       <c r="B26" s="41" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
@@ -2731,7 +2730,7 @@
       <c r="F26" s="9"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="55"/>
+      <c r="A27" s="56"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
@@ -2764,7 +2763,7 @@
       <c r="A32" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="44" t="s">
+      <c r="B32" s="43" t="s">
         <v>80</v>
       </c>
       <c r="C32" s="4"/>
@@ -2776,8 +2775,8 @@
       <c r="A33" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="57" t="s">
-        <v>89</v>
+      <c r="B33" s="51" t="s">
+        <v>88</v>
       </c>
       <c r="C33" s="20"/>
       <c r="D33" s="20"/>
@@ -2871,7 +2870,7 @@
       <c r="A46" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B46" s="44" t="s">
+      <c r="B46" s="43" t="s">
         <v>81</v>
       </c>
       <c r="C46" s="4"/>
@@ -2883,8 +2882,8 @@
       <c r="A47" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B47" s="57" t="s">
-        <v>90</v>
+      <c r="B47" s="51" t="s">
+        <v>89</v>
       </c>
       <c r="C47" s="20"/>
       <c r="D47" s="20"/>
@@ -2978,7 +2977,7 @@
       <c r="A61" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B61" s="44" t="s">
+      <c r="B61" s="43" t="s">
         <v>82</v>
       </c>
       <c r="C61" s="4"/>
@@ -2990,8 +2989,8 @@
       <c r="A62" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B62" s="57" t="s">
-        <v>91</v>
+      <c r="B62" s="51" t="s">
+        <v>90</v>
       </c>
       <c r="C62" s="20"/>
       <c r="D62" s="20"/>
@@ -3043,6 +3042,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A11" r:id="rId1" xr:uid="{5FDCBA1E-2181-224B-8606-C4BBFE30E740}"/>
+    <hyperlink ref="A12" r:id="rId2" xr:uid="{8A08332E-F497-D648-9C95-62E6A69B1966}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>